<commit_message>
ran through code for month of July. Got it all to work.
</commit_message>
<xml_diff>
--- a/Month-over-Month_change_log_Table.xlsx
+++ b/Month-over-Month_change_log_Table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,7 +544,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>purdueprofessors</t>
+          <t>stanfordprofessors</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -554,17 +554,17 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Addition</t>
+          <t>Deletion</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Xiaoping Du</t>
+          <t>Drew Nelson</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Professor of Mechanical Engineering (Indianapolis)</t>
+          <t>Professor of Mechanical Engineering</t>
         </is>
       </c>
     </row>
@@ -635,24 +635,24 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Deletion</t>
+          <t>Addition</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Weinong Chen</t>
+          <t>Xiaoping Du</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Reilly Professor of Aeronautics and Astronautics &amp; Materials Engineering; Professor of Mechanical Engineering (by Courtesy)</t>
+          <t>Professor of Mechanical Engineering (Indianapolis)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>stanfordprofessors</t>
+          <t>purdueprofessors</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -667,12 +667,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Drew Nelson</t>
+          <t>Weinong Chen</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Professor of Mechanical Engineering</t>
+          <t>Reilly Professor of Aeronautics and Astronautics &amp; Materials Engineering; Professor of Mechanical Engineering (by Courtesy)</t>
         </is>
       </c>
     </row>
@@ -721,7 +721,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Robert Dibble</t>
+          <t>Ralph Greif</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -748,7 +748,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Ralph Greif</t>
+          <t>Robert Dibble</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -775,12 +775,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Chia-Fon  Lee</t>
+          <t>Ann Sychterz</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Assistant Professor</t>
         </is>
       </c>
     </row>
@@ -802,12 +802,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Theresa Ann Saxton-Fox</t>
+          <t>Chia-Fon  Lee</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Asst Professor</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -829,12 +829,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Ann Sychterz</t>
+          <t>Theresa Ann Saxton-Fox</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Assistant Professor</t>
+          <t>Asst Professor</t>
         </is>
       </c>
     </row>
@@ -895,7 +895,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>georgiaprofessors</t>
+          <t>michiganprofessors</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -905,24 +905,24 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Deletion</t>
+          <t>Addition</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Yan Wang</t>
+          <t>Art Hyde</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Associate Professor of Engineering Practice, Mechanical Engineering</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>georgiaprofessors</t>
+          <t>michiganprofessors</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -932,24 +932,24 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Deletion</t>
+          <t>Addition</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>C.-K. Chris Wang</t>
+          <t>Jason Siegel</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Research Associate Professor, Mechanical Engineering</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>georgiaprofessors</t>
+          <t>michiganprofessors</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -959,24 +959,24 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Deletion</t>
+          <t>Addition</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>C.-K. Chris Wang</t>
+          <t>Martin Erinin</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Assistant Professor (Joining January 2025), Mechanical Engineering</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>michiganprofessors</t>
+          <t>UIUCprofessors</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -991,19 +991,19 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Martin Erinin</t>
+          <t>C. Ricardo Constante Amores</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Assistant Professor (Joining January 2025), Mechanical Engineering</t>
+          <t>Assistant Professor, starting August 2024</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>michiganprofessors</t>
+          <t>UIUCprofessors</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1018,19 +1018,19 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Art Hyde</t>
+          <t>Nazanin  Farjam</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Associate Professor of Engineering Practice, Mechanical Engineering</t>
+          <t>Assistant Professor, starting August 2024</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>michiganprofessors</t>
+          <t>UIUCprofessors</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1040,24 +1040,24 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Addition</t>
+          <t>Deletion</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Jason Siegel</t>
+          <t>Alex Vakakis</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Research Associate Professor, Mechanical Engineering</t>
+          <t>Donald Biggar Willett Professor</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>purdueprofessors</t>
+          <t>UIUCprofessors</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1067,24 +1067,24 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Addition</t>
+          <t>Deletion</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Jie Cai</t>
+          <t>Amy  Wagoner Johnson</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Associate Professor of Mechanical Engineering</t>
+          <t>Professor; Andersen Faculty Scholar</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>purdueprofessors</t>
+          <t>UIUCprofessors</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1094,24 +1094,24 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Addition</t>
+          <t>Deletion</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Razi Nalim</t>
+          <t>Ann Sychterz</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Professor of Mechanical Engineering (Purdue University in Indianapolis, by courtesy)</t>
+          <t>Assistant Professor</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>purdueprofessors</t>
+          <t>UIUCprofessors</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1126,19 +1126,19 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Bumsoo Han</t>
+          <t>Arend  van der Zande</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Professor of Mechanical Engineering, and Professor of Biomedical Engineering (by Courtesy)</t>
+          <t>Associate Professor</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>purdueprofessors</t>
+          <t>UIUCprofessors</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1153,19 +1153,19 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Eric Adams</t>
+          <t>Arif  Masud</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Associate Professor of Engineering Practice (Indianapolis)</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>purdueprofessors</t>
+          <t>UIUCprofessors</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1180,12 +1180,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Mohamed Nalim</t>
+          <t>Arne J. Pearlstein</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Professor of Mechanical Engineering (Purdue University in Indianapolis, by courtesy)</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -1202,17 +1202,17 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Addition</t>
+          <t>Deletion</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>C. Ricardo Constante Amores</t>
+          <t>Bill King</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Assistant Professor, starting August 2024</t>
+          <t>Ralph A. Andersen Endowed Chair; Faculty at Carle Illinois College of Medicine</t>
         </is>
       </c>
     </row>
@@ -1229,17 +1229,17 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Addition</t>
+          <t>Deletion</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Nazanin  Farjam</t>
+          <t>Callan Luetkemeyer</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Assistant Professor, starting August 2024</t>
+          <t>Assistant Professor</t>
         </is>
       </c>
     </row>
@@ -1261,12 +1261,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Kris K. Hauser</t>
+          <t>Chia-Fon  Lee</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Associate Professor</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -1288,12 +1288,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Sascha  Hilgenfeldt</t>
+          <t>Dusan M. Stipanovic</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Professor; Willett Faculty Scholar</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -1315,12 +1315,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Naira Hovakimyan</t>
+          <t>Elizabeth T. Hsiao-Wecksler</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>W. Grafton and Lillian B. Wilkins Professor; University Scholar; Schaller Faculty Scholar</t>
+          <t>Grayce Wicall Gauthier Professor</t>
         </is>
       </c>
     </row>
@@ -1342,12 +1342,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Elizabeth T. Hsiao-Wecksler</t>
+          <t>Francesco  Panerai</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Grayce Wicall Gauthier Professor</t>
+          <t>Assistant Professor</t>
         </is>
       </c>
     </row>
@@ -1369,12 +1369,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Shelby  Hutchens</t>
+          <t>Gabriel  Juarez</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Associate Professor</t>
+          <t>Assistant Professor</t>
         </is>
       </c>
     </row>
@@ -1396,12 +1396,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Tony Jacobi</t>
+          <t>Girish  Krishnan</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Department Head, Richard W. Kritzer Distinguished Professor</t>
+          <t>ASST PROF</t>
         </is>
       </c>
     </row>
@@ -1423,12 +1423,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Iwona M. Jasiuk</t>
+          <t>Harley T. Johnson</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Professor; Richard W. Kritzer Faculty Scholar</t>
+          <t>Founder Professor; Associate Dean for Research, The Grainger College of Engineering</t>
         </is>
       </c>
     </row>
@@ -1450,12 +1450,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Harley T. Johnson</t>
+          <t>Huseyin  Sehitoglu</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Founder Professor; Associate Dean for Research, The Grainger College of Engineering</t>
+          <t>Professor; John, Alice and Sarah Nyquist Chair</t>
         </is>
       </c>
     </row>
@@ -1477,12 +1477,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Gabriel  Juarez</t>
+          <t>Iwona M. Jasiuk</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Assistant Professor</t>
+          <t>Professor; Richard W. Kritzer Faculty Scholar</t>
         </is>
       </c>
     </row>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Paul J. A. Kenis</t>
+          <t>Jeff Shamma</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1531,12 +1531,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Mariana E. Kersh</t>
+          <t>Joao Ramos</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Associate Professor</t>
+          <t>Assistant Professor</t>
         </is>
       </c>
     </row>
@@ -1558,12 +1558,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Joohyung  Kim</t>
+          <t>John  Lambros</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Associate Professor</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -1585,12 +1585,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Bill King</t>
+          <t>John S. Popovics</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Ralph A. Andersen Endowed Chair; Faculty at Carle Illinois College of Medicine</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -1612,12 +1612,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Seid  Koric</t>
+          <t>Joohyung  Kim</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Research Associate Professor</t>
+          <t>Associate Professor</t>
         </is>
       </c>
     </row>
@@ -1639,12 +1639,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Girish  Krishnan</t>
+          <t>Justin Yim</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>ASST PROF</t>
+          <t>Assistant Professor</t>
         </is>
       </c>
     </row>
@@ -1666,12 +1666,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Waltraud M. Kriven</t>
+          <t>Kathryn  Matlack</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Associate Professor; Richard W. Kritzer Faculty Scholar</t>
         </is>
       </c>
     </row>
@@ -1693,12 +1693,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>John  Lambros</t>
+          <t>Kelly  Stephani</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Associate Professor; Kritzer Faculty Fellow</t>
         </is>
       </c>
     </row>
@@ -1720,12 +1720,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Chia-Fon  Lee</t>
+          <t>Kris K. Hauser</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Associate Professor</t>
         </is>
       </c>
     </row>
@@ -1747,12 +1747,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Tonghun  Lee</t>
+          <t>Kyle Smith</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Bei Tse Chao and May Chao Professor</t>
+          <t>Associate Professor</t>
         </is>
       </c>
     </row>
@@ -1774,12 +1774,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Xiuling  Li</t>
+          <t>M Taher A. Saif</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Edward William and Jane Marr Gutgsell Professor</t>
         </is>
       </c>
     </row>
@@ -1801,12 +1801,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Callan Luetkemeyer</t>
+          <t>Marco  Panesi</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Assistant Professor</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -1828,12 +1828,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Arif  Masud</t>
+          <t>Mariana E. Kersh</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Associate Professor</t>
         </is>
       </c>
     </row>
@@ -1855,12 +1855,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Moshe Matalon</t>
+          <t>Martin  Ostoja-Starzewski</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Caterpillar Distinguished Professor</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -1882,12 +1882,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Kathryn  Matlack</t>
+          <t>Matthew  West</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Associate Professor; Richard W. Kritzer Faculty Scholar</t>
+          <t>Professor; William H. Severns Faculty Scholar</t>
         </is>
       </c>
     </row>
@@ -1909,12 +1909,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Prashant Mehta</t>
+          <t>Moshe Matalon</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Caterpillar Distinguished Professor</t>
         </is>
       </c>
     </row>
@@ -1936,12 +1936,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Nenad  Miljkovic</t>
+          <t>Naira Hovakimyan</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Founder Professor; Director, ACRC</t>
+          <t>W. Grafton and Lillian B. Wilkins Professor; University Scholar; Schaller Faculty Scholar</t>
         </is>
       </c>
     </row>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Martin  Ostoja-Starzewski</t>
+          <t>Nancy R. Sottos</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1990,12 +1990,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Francesco  Panerai</t>
+          <t>Nenad  Miljkovic</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Assistant Professor</t>
+          <t>Founder Professor; Director, ACRC</t>
         </is>
       </c>
     </row>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Marco  Panesi</t>
+          <t>Paul J. A. Kenis</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2044,12 +2044,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Arne J. Pearlstein</t>
+          <t>Petros  Sofronis</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>James W. Bayne Professor; Director, International Institute for Carbon-Neutral Energy Research</t>
         </is>
       </c>
     </row>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>John S. Popovics</t>
+          <t>Prashant Mehta</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2098,12 +2098,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Joao Ramos</t>
+          <t>Sameh Tawfick</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Assistant Professor</t>
+          <t>Associate Professor; Ralph A. Andersen Faculty Scholar</t>
         </is>
       </c>
     </row>
@@ -2125,12 +2125,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>M Taher A. Saif</t>
+          <t>Sanjiv  Sinha</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Edward William and Jane Marr Gutgsell Professor</t>
+          <t>Professor; Associate Head for Undergraduate Programs</t>
         </is>
       </c>
     </row>
@@ -2152,12 +2152,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Srinivasa M. Salapaka</t>
+          <t>Sascha  Hilgenfeldt</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Professor; Willett Faculty Scholar</t>
         </is>
       </c>
     </row>
@@ -2179,12 +2179,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Theresa Ann Saxton-Fox</t>
+          <t>Seid  Koric</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Asst Professor</t>
+          <t>Research Associate Professor</t>
         </is>
       </c>
     </row>
@@ -2206,12 +2206,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Huseyin  Sehitoglu</t>
+          <t>Shelby  Hutchens</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Professor; John, Alice and Sarah Nyquist Chair</t>
+          <t>Associate Professor</t>
         </is>
       </c>
     </row>
@@ -2233,12 +2233,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Jeff Shamma</t>
+          <t>Siyi  Xu</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Assistant Professor, starting August 2024</t>
         </is>
       </c>
     </row>
@@ -2260,12 +2260,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Sanjiv  Sinha</t>
+          <t>Sophie  Wang</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Professor; Associate Head for Undergraduate Programs</t>
+          <t>Research Associate Professor</t>
         </is>
       </c>
     </row>
@@ -2287,12 +2287,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Kyle Smith</t>
+          <t>Srinivasa M. Salapaka</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Associate Professor</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -2314,12 +2314,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Petros  Sofronis</t>
+          <t>Theresa Ann Saxton-Fox</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>James W. Bayne Professor; Director, International Institute for Carbon-Neutral Energy Research</t>
+          <t>Asst Professor</t>
         </is>
       </c>
     </row>
@@ -2341,12 +2341,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Nancy R. Sottos</t>
+          <t>Tonghun  Lee</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Bei Tse Chao and May Chao Professor</t>
         </is>
       </c>
     </row>
@@ -2368,12 +2368,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Kelly  Stephani</t>
+          <t>Tony Jacobi</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Associate Professor; Kritzer Faculty Fellow</t>
+          <t>Department Head, Richard W. Kritzer Distinguished Professor</t>
         </is>
       </c>
     </row>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Dusan M. Stipanovic</t>
+          <t>Waltraud M. Kriven</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2422,12 +2422,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Ann Sychterz</t>
+          <t>Xinlei  Wang</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Assistant Professor</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -2449,12 +2449,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Sameh Tawfick</t>
+          <t>Xiuling  Li</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Associate Professor; Ralph A. Andersen Faculty Scholar</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
@@ -2476,19 +2476,19 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>Alex Vakakis</t>
+          <t>Yuanhui  Zhang</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Donald Biggar Willett Professor</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>UIUCprofessors</t>
+          <t>georgiaprofessors</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2503,19 +2503,19 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Arend  van der Zande</t>
+          <t>C.-K. Chris Wang</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Associate Professor</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>UIUCprofessors</t>
+          <t>georgiaprofessors</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2530,19 +2530,19 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Amy  Wagoner Johnson</t>
+          <t>C.-K. Chris Wang</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Professor; Andersen Faculty Scholar</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>UIUCprofessors</t>
+          <t>georgiaprofessors</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2557,19 +2557,19 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Sophie  Wang</t>
+          <t>Yan Wang</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Research Associate Professor</t>
+          <t>Professor</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>UIUCprofessors</t>
+          <t>purdueprofessors</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2579,24 +2579,24 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Deletion</t>
+          <t>Addition</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Xinlei  Wang</t>
+          <t>Jie Cai</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Professor</t>
+          <t>Associate Professor of Mechanical Engineering</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>UIUCprofessors</t>
+          <t>purdueprofessors</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2606,24 +2606,24 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Deletion</t>
+          <t>Addition</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>Matthew  West</t>
+          <t>Razi Nalim</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Professor; William H. Severns Faculty Scholar</t>
+          <t>Professor of Mechanical Engineering (Purdue University in Indianapolis, by courtesy)</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>UIUCprofessors</t>
+          <t>purdueprofessors</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2638,19 +2638,19 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Siyi  Xu</t>
+          <t>Bumsoo Han</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Assistant Professor, starting August 2024</t>
+          <t>Professor of Mechanical Engineering, and Professor of Biomedical Engineering (by Courtesy)</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>UIUCprofessors</t>
+          <t>purdueprofessors</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2665,19 +2665,19 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Justin Yim</t>
+          <t>Eric Adams</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Assistant Professor</t>
+          <t>Associate Professor of Engineering Practice (Indianapolis)</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>UIUCprofessors</t>
+          <t>purdueprofessors</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2692,12 +2692,1686 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
+          <t>Mohamed Nalim</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Professor of Mechanical Engineering (Purdue University in Indianapolis, by courtesy)</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>mitprofessors</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Deletion</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Gopinath, Ashwin</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>Assistant Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>mitprofessors</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Deletion</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Rodriguez Garcia, Alberto</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Associate Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>stanfordprofessors</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Adam Meyer Boies</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Associate Professor of Mechanical Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Alex Vakakis</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Donald Biggar Willett Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Amy  Wagoner Johnson</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Professor; Andersen Faculty Scholar</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Ann Sychterz</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Assistant Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Arend  van der Zande</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Associate Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Arif  Masud</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Arne J. Pearlstein</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Bill King</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>Ralph A. Andersen Endowed Chair; Faculty at Carle Illinois College of Medicine</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>C. Ricardo Constante-Amores</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Assistant Professor, starting August 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Callan Luetkemeyer</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Assistant Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Chia-Fon  Lee</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Dusan M. Stipanovic</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Elizabeth T. Hsiao-Wecksler</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Grayce Wicall Gauthier Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Francesco  Panerai</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Assistant Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Gabriel  Juarez</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Assistant Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Girish  Krishnan</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>ASST PROF</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Harley T. Johnson</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>Founder Professor; Associate Dean for Research, The Grainger College of Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Huseyin  Sehitoglu</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Professor; John, Alice and Sarah Nyquist Chair</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Iwona M. Jasiuk</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Professor; Richard W. Kritzer Faculty Scholar</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Jeff Shamma</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Joao Ramos</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Assistant Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>John  Lambros</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>John S. Popovics</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Joohyung  Kim</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Associate Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Justin Yim</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Assistant Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Kathryn  Matlack</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Associate Professor; Richard W. Kritzer Faculty Scholar</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Kelly  Stephani</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Associate Professor; Kritzer Faculty Fellow</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Kris K. Hauser</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Associate Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Kyle Smith</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Associate Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>M Taher A. Saif</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Edward William and Jane Marr Gutgsell Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Marco  Panesi</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Mariana E. Kersh</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Associate Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Martin  Ostoja-Starzewski</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Matthew  West</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Professor; William H. Severns Faculty Scholar</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Moshe Matalon</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Caterpillar Distinguished Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Naira Hovakimyan</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>W. Grafton and Lillian B. Wilkins Professor; University Scholar; Schaller Faculty Scholar</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Nancy R. Sottos</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Nenad  Miljkovic</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Founder Professor; Director, ACRC</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Paul J. A. Kenis</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Petros  Sofronis</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>James W. Bayne Professor; Director, International Institute for Carbon-Neutral Energy Research</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Prashant Mehta</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Sameh Tawfick</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Associate Professor; Ralph A. Andersen Faculty Scholar</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Sanjiv  Sinha</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Professor; Associate Head for Undergraduate Programs</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Sascha  Hilgenfeldt</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Professor; Willett Faculty Scholar</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Seid  Koric</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Research Associate Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Shelby  Hutchens</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Associate Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Siyi  Xu</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Assistant Professor, starting August 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Sophie  Wang</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Research Associate Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Srinivasa M. Salapaka</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Theresa Ann Saxton-Fox</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Asst Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Tonghun  Lee</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Bei Tse Chao and May Chao Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Tony Jacobi</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Department Head, Richard W. Kritzer Distinguished Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Waltraud M. Kriven</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Xinlei  Wang</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Xiuling  Li</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
           <t>Yuanhui  Zhang</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="E142" t="inlineStr">
         <is>
           <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>Deletion</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>C. Ricardo Constante Amores</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Assistant Professor, starting August 2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>georgiaprofessors</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>C.-K. Chris Wang</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>georgiaprofessors</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Yan Wang</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>georgiaprofessors</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>Deletion</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Zhuomin Zhang</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>J. Erskine Love, Jr. Professor</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update for month of October
</commit_message>
<xml_diff>
--- a/Month-over-Month_change_log_Table.xlsx
+++ b/Month-over-Month_change_log_Table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1866,6 +1866,222 @@
         </is>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>mitprofessors</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Zufferey, Raphael</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Assistant Professor (Starting January 2025)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>michiganprofessors</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Jacinto Ulloa</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Assistant Professor, Mechanical Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>michiganprofessors</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Deletion</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Jesse Austin-Breneman</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Assistant Professor, Mechanical Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Anthony Jacobi</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Department Head, Richard W. Kritzer Distinguished Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Cunjiang Yu</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Founder Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>UIUCprofessors</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Deletion</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Tony Jacobi</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Department Head, Richard W. Kritzer Distinguished Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>georgiaprofessors</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Christopher J. Saldaña</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Ring Family Professor</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>georgiaprofessors</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Addition</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Samuel Graham</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>